<commit_message>
Changed init for sharepoint and queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\UiPath\P0001_090_PayCycleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2449A172-9BB7-4717-93CD-28DBA69D7385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B3EF43-26B4-4C3C-8C1B-5932A2A239DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -85,10 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
@@ -174,9 +170,6 @@
     <t>This error occurs when the process monitor table does not have any rows.</t>
   </si>
   <si>
-    <t>State wide Accounting - Pay Cycle Queries</t>
-  </si>
-  <si>
     <t>DownloadFolderPath</t>
   </si>
   <si>
@@ -201,12 +194,6 @@
     <t>VoucherQueueName</t>
   </si>
   <si>
-    <t>SWA_PayCycleQueries_Vouchers</t>
-  </si>
-  <si>
-    <t>SWA_PayCycleQueries_Queries</t>
-  </si>
-  <si>
     <t>Query2</t>
   </si>
   <si>
@@ -313,6 +300,117 @@
   </si>
   <si>
     <t>Manual Query</t>
+  </si>
+  <si>
+    <t>Name of the Sharepoint Bot folder</t>
+  </si>
+  <si>
+    <t>Path to the folder till Date folder. This should be kept empty in the config</t>
+  </si>
+  <si>
+    <t>SharepointBotFolderPath</t>
+  </si>
+  <si>
+    <t>SharepointManualFolderPath</t>
+  </si>
+  <si>
+    <t>Name of the Tenant ID Asset</t>
+  </si>
+  <si>
+    <t>Name of the App ID Asset</t>
+  </si>
+  <si>
+    <t>Name of the App Secret Asset</t>
+  </si>
+  <si>
+    <t>Pay Cycle Queries</t>
+  </si>
+  <si>
+    <t>SE2</t>
+  </si>
+  <si>
+    <t>Sharepoint sub folder is not available</t>
+  </si>
+  <si>
+    <t>MorningStartTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_MorningRun_StartTime</t>
+  </si>
+  <si>
+    <t>MorningEndTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_MorningRun_EndTime</t>
+  </si>
+  <si>
+    <t>NoonStartTime</t>
+  </si>
+  <si>
+    <t>NoonEndTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_NoonRun_StartTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_NoonRun_EndTime</t>
+  </si>
+  <si>
+    <t>EveningStartTime</t>
+  </si>
+  <si>
+    <t>EveningEndTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_EveningRun_StartTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_EveningRun_EndTime</t>
+  </si>
+  <si>
+    <t>Date time for Morning run</t>
+  </si>
+  <si>
+    <t>Date time for Noon run</t>
+  </si>
+  <si>
+    <t>Date time for Evening run</t>
+  </si>
+  <si>
+    <t>ProcessMonitorDuration</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ProcessMonitorDuration</t>
+  </si>
+  <si>
+    <t>Interval to set in process monitor fields</t>
+  </si>
+  <si>
+    <t>ProcessMonitorUser</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ProcessMonitorUser</t>
+  </si>
+  <si>
+    <t>UserID for Process Monitor fields</t>
+  </si>
+  <si>
+    <t>ProcessMonitorDurationType</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ProcessMonitorDurationType</t>
+  </si>
+  <si>
+    <t>Duration type (Days, Weeks, Years)</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Voucher</t>
+  </si>
+  <si>
+    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
   </si>
 </sst>
 </file>
@@ -689,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -739,31 +837,33 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="45">
       <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -772,1332 +872,149 @@
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
         <v>92</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z996"/>
-  <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="30">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="45">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:3" ht="45">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3">
+        <v>78</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3">
+        <v>79</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
-      </c>
-    </row>
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3067,26 +1984,32 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3094,14 +2017,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -3125,89 +2046,1416 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
+    <row r="2" spans="1:26" ht="30">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="45">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="45">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
+    <row r="798" ht="14.25" customHeight="1"/>
+    <row r="799" ht="14.25" customHeight="1"/>
+    <row r="800" ht="14.25" customHeight="1"/>
+    <row r="801" ht="14.25" customHeight="1"/>
+    <row r="802" ht="14.25" customHeight="1"/>
+    <row r="803" ht="14.25" customHeight="1"/>
+    <row r="804" ht="14.25" customHeight="1"/>
+    <row r="805" ht="14.25" customHeight="1"/>
+    <row r="806" ht="14.25" customHeight="1"/>
+    <row r="807" ht="14.25" customHeight="1"/>
+    <row r="808" ht="14.25" customHeight="1"/>
+    <row r="809" ht="14.25" customHeight="1"/>
+    <row r="810" ht="14.25" customHeight="1"/>
+    <row r="811" ht="14.25" customHeight="1"/>
+    <row r="812" ht="14.25" customHeight="1"/>
+    <row r="813" ht="14.25" customHeight="1"/>
+    <row r="814" ht="14.25" customHeight="1"/>
+    <row r="815" ht="14.25" customHeight="1"/>
+    <row r="816" ht="14.25" customHeight="1"/>
+    <row r="817" ht="14.25" customHeight="1"/>
+    <row r="818" ht="14.25" customHeight="1"/>
+    <row r="819" ht="14.25" customHeight="1"/>
+    <row r="820" ht="14.25" customHeight="1"/>
+    <row r="821" ht="14.25" customHeight="1"/>
+    <row r="822" ht="14.25" customHeight="1"/>
+    <row r="823" ht="14.25" customHeight="1"/>
+    <row r="824" ht="14.25" customHeight="1"/>
+    <row r="825" ht="14.25" customHeight="1"/>
+    <row r="826" ht="14.25" customHeight="1"/>
+    <row r="827" ht="14.25" customHeight="1"/>
+    <row r="828" ht="14.25" customHeight="1"/>
+    <row r="829" ht="14.25" customHeight="1"/>
+    <row r="830" ht="14.25" customHeight="1"/>
+    <row r="831" ht="14.25" customHeight="1"/>
+    <row r="832" ht="14.25" customHeight="1"/>
+    <row r="833" ht="14.25" customHeight="1"/>
+    <row r="834" ht="14.25" customHeight="1"/>
+    <row r="835" ht="14.25" customHeight="1"/>
+    <row r="836" ht="14.25" customHeight="1"/>
+    <row r="837" ht="14.25" customHeight="1"/>
+    <row r="838" ht="14.25" customHeight="1"/>
+    <row r="839" ht="14.25" customHeight="1"/>
+    <row r="840" ht="14.25" customHeight="1"/>
+    <row r="841" ht="14.25" customHeight="1"/>
+    <row r="842" ht="14.25" customHeight="1"/>
+    <row r="843" ht="14.25" customHeight="1"/>
+    <row r="844" ht="14.25" customHeight="1"/>
+    <row r="845" ht="14.25" customHeight="1"/>
+    <row r="846" ht="14.25" customHeight="1"/>
+    <row r="847" ht="14.25" customHeight="1"/>
+    <row r="848" ht="14.25" customHeight="1"/>
+    <row r="849" ht="14.25" customHeight="1"/>
+    <row r="850" ht="14.25" customHeight="1"/>
+    <row r="851" ht="14.25" customHeight="1"/>
+    <row r="852" ht="14.25" customHeight="1"/>
+    <row r="853" ht="14.25" customHeight="1"/>
+    <row r="854" ht="14.25" customHeight="1"/>
+    <row r="855" ht="14.25" customHeight="1"/>
+    <row r="856" ht="14.25" customHeight="1"/>
+    <row r="857" ht="14.25" customHeight="1"/>
+    <row r="858" ht="14.25" customHeight="1"/>
+    <row r="859" ht="14.25" customHeight="1"/>
+    <row r="860" ht="14.25" customHeight="1"/>
+    <row r="861" ht="14.25" customHeight="1"/>
+    <row r="862" ht="14.25" customHeight="1"/>
+    <row r="863" ht="14.25" customHeight="1"/>
+    <row r="864" ht="14.25" customHeight="1"/>
+    <row r="865" ht="14.25" customHeight="1"/>
+    <row r="866" ht="14.25" customHeight="1"/>
+    <row r="867" ht="14.25" customHeight="1"/>
+    <row r="868" ht="14.25" customHeight="1"/>
+    <row r="869" ht="14.25" customHeight="1"/>
+    <row r="870" ht="14.25" customHeight="1"/>
+    <row r="871" ht="14.25" customHeight="1"/>
+    <row r="872" ht="14.25" customHeight="1"/>
+    <row r="873" ht="14.25" customHeight="1"/>
+    <row r="874" ht="14.25" customHeight="1"/>
+    <row r="875" ht="14.25" customHeight="1"/>
+    <row r="876" ht="14.25" customHeight="1"/>
+    <row r="877" ht="14.25" customHeight="1"/>
+    <row r="878" ht="14.25" customHeight="1"/>
+    <row r="879" ht="14.25" customHeight="1"/>
+    <row r="880" ht="14.25" customHeight="1"/>
+    <row r="881" ht="14.25" customHeight="1"/>
+    <row r="882" ht="14.25" customHeight="1"/>
+    <row r="883" ht="14.25" customHeight="1"/>
+    <row r="884" ht="14.25" customHeight="1"/>
+    <row r="885" ht="14.25" customHeight="1"/>
+    <row r="886" ht="14.25" customHeight="1"/>
+    <row r="887" ht="14.25" customHeight="1"/>
+    <row r="888" ht="14.25" customHeight="1"/>
+    <row r="889" ht="14.25" customHeight="1"/>
+    <row r="890" ht="14.25" customHeight="1"/>
+    <row r="891" ht="14.25" customHeight="1"/>
+    <row r="892" ht="14.25" customHeight="1"/>
+    <row r="893" ht="14.25" customHeight="1"/>
+    <row r="894" ht="14.25" customHeight="1"/>
+    <row r="895" ht="14.25" customHeight="1"/>
+    <row r="896" ht="14.25" customHeight="1"/>
+    <row r="897" ht="14.25" customHeight="1"/>
+    <row r="898" ht="14.25" customHeight="1"/>
+    <row r="899" ht="14.25" customHeight="1"/>
+    <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25" customHeight="1"/>
+    <row r="903" ht="14.25" customHeight="1"/>
+    <row r="904" ht="14.25" customHeight="1"/>
+    <row r="905" ht="14.25" customHeight="1"/>
+    <row r="906" ht="14.25" customHeight="1"/>
+    <row r="907" ht="14.25" customHeight="1"/>
+    <row r="908" ht="14.25" customHeight="1"/>
+    <row r="909" ht="14.25" customHeight="1"/>
+    <row r="910" ht="14.25" customHeight="1"/>
+    <row r="911" ht="14.25" customHeight="1"/>
+    <row r="912" ht="14.25" customHeight="1"/>
+    <row r="913" ht="14.25" customHeight="1"/>
+    <row r="914" ht="14.25" customHeight="1"/>
+    <row r="915" ht="14.25" customHeight="1"/>
+    <row r="916" ht="14.25" customHeight="1"/>
+    <row r="917" ht="14.25" customHeight="1"/>
+    <row r="918" ht="14.25" customHeight="1"/>
+    <row r="919" ht="14.25" customHeight="1"/>
+    <row r="920" ht="14.25" customHeight="1"/>
+    <row r="921" ht="14.25" customHeight="1"/>
+    <row r="922" ht="14.25" customHeight="1"/>
+    <row r="923" ht="14.25" customHeight="1"/>
+    <row r="924" ht="14.25" customHeight="1"/>
+    <row r="925" ht="14.25" customHeight="1"/>
+    <row r="926" ht="14.25" customHeight="1"/>
+    <row r="927" ht="14.25" customHeight="1"/>
+    <row r="928" ht="14.25" customHeight="1"/>
+    <row r="929" ht="14.25" customHeight="1"/>
+    <row r="930" ht="14.25" customHeight="1"/>
+    <row r="931" ht="14.25" customHeight="1"/>
+    <row r="932" ht="14.25" customHeight="1"/>
+    <row r="933" ht="14.25" customHeight="1"/>
+    <row r="934" ht="14.25" customHeight="1"/>
+    <row r="935" ht="14.25" customHeight="1"/>
+    <row r="936" ht="14.25" customHeight="1"/>
+    <row r="937" ht="14.25" customHeight="1"/>
+    <row r="938" ht="14.25" customHeight="1"/>
+    <row r="939" ht="14.25" customHeight="1"/>
+    <row r="940" ht="14.25" customHeight="1"/>
+    <row r="941" ht="14.25" customHeight="1"/>
+    <row r="942" ht="14.25" customHeight="1"/>
+    <row r="943" ht="14.25" customHeight="1"/>
+    <row r="944" ht="14.25" customHeight="1"/>
+    <row r="945" ht="14.25" customHeight="1"/>
+    <row r="946" ht="14.25" customHeight="1"/>
+    <row r="947" ht="14.25" customHeight="1"/>
+    <row r="948" ht="14.25" customHeight="1"/>
+    <row r="949" ht="14.25" customHeight="1"/>
+    <row r="950" ht="14.25" customHeight="1"/>
+    <row r="951" ht="14.25" customHeight="1"/>
+    <row r="952" ht="14.25" customHeight="1"/>
+    <row r="953" ht="14.25" customHeight="1"/>
+    <row r="954" ht="14.25" customHeight="1"/>
+    <row r="955" ht="14.25" customHeight="1"/>
+    <row r="956" ht="14.25" customHeight="1"/>
+    <row r="957" ht="14.25" customHeight="1"/>
+    <row r="958" ht="14.25" customHeight="1"/>
+    <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
+    <row r="962" ht="14.25" customHeight="1"/>
+    <row r="963" ht="14.25" customHeight="1"/>
+    <row r="964" ht="14.25" customHeight="1"/>
+    <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
+    <row r="975" ht="14.25" customHeight="1"/>
+    <row r="976" ht="14.25" customHeight="1"/>
+    <row r="977" ht="14.25" customHeight="1"/>
+    <row r="978" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
+    <row r="982" ht="14.25" customHeight="1"/>
+    <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
+    <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z997"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>74</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -4191,9 +4439,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Kill process proprties to Current user. Made minor adjustment to exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB170FC-0083-4FFB-8CDD-1CA437E5E39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415658C8-8297-44CD-8710-0833F61C6D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="220">
   <si>
     <t>Name</t>
   </si>
@@ -89,11 +89,11 @@
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="12"/>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="12"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -168,54 +168,15 @@
     <t>DownloadFileExtension</t>
   </si>
   <si>
-    <t>Query1</t>
-  </si>
-  <si>
-    <t>PJG_AO_VOUCHERS</t>
-  </si>
-  <si>
     <t>VoucherQueueName</t>
   </si>
   <si>
-    <t>Query2</t>
-  </si>
-  <si>
-    <t>Query3</t>
-  </si>
-  <si>
-    <t>Query4</t>
-  </si>
-  <si>
-    <t>Query5</t>
-  </si>
-  <si>
-    <t>Query6</t>
-  </si>
-  <si>
-    <t>CIW_EFT_7EFT_NO_BANK_FLAG_7</t>
-  </si>
-  <si>
-    <t>CH_VCHRS_INVALID_PAY_GROUP_7</t>
-  </si>
-  <si>
-    <t>PJG_BIU_AGENCY_VOUCHERS</t>
-  </si>
-  <si>
-    <t>CH_AGY_WRRNT_PYMNTS</t>
-  </si>
-  <si>
-    <t>PCARD_PAYGROUP_CH</t>
-  </si>
-  <si>
     <t>SharepointURL</t>
   </si>
   <si>
     <t>P001_090_PayCycleQueries_SharepointURL</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>P001_090_PayCycleQueries_PeoplesoftURL</t>
   </si>
   <si>
@@ -252,18 +213,9 @@
     <t>BotFolderName</t>
   </si>
   <si>
-    <t>Bot Query</t>
-  </si>
-  <si>
     <t>ManualFolderName</t>
   </si>
   <si>
-    <t>Manual Query</t>
-  </si>
-  <si>
-    <t>Name of the Sharepoint Bot folder</t>
-  </si>
-  <si>
     <t>Path to the folder till Date folder. This should be kept empty in the config</t>
   </si>
   <si>
@@ -411,54 +363,30 @@
     <t>Exception Type</t>
   </si>
   <si>
-    <t>Bot Responsibility</t>
-  </si>
-  <si>
     <t>Notification Type</t>
   </si>
   <si>
-    <t>Timing of Notification</t>
-  </si>
-  <si>
     <t>SE_1</t>
   </si>
   <si>
-    <t>PeopleSoft application unavailable</t>
-  </si>
-  <si>
     <t>System Exception</t>
   </si>
   <si>
-    <t>Perform the process manually</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>At the time of exception</t>
-  </si>
-  <si>
     <t>Business Team</t>
   </si>
   <si>
-    <t>Retry 3 times before erroring out</t>
-  </si>
-  <si>
     <t>SE_2</t>
   </si>
   <si>
-    <t>PeopleSoft login failed</t>
-  </si>
-  <si>
     <t>BE_1</t>
   </si>
   <si>
     <t>Business Exception</t>
   </si>
   <si>
-    <t>Queries unavailable in Peoplesoft</t>
-  </si>
-  <si>
     <t>BE_2</t>
   </si>
   <si>
@@ -472,15 +400,6 @@
   </si>
   <si>
     <t>BE_4</t>
-  </si>
-  <si>
-    <t>BE_5</t>
-  </si>
-  <si>
-    <t>Bot:
-- Take screenshot
--  Send notification to business &amp; support team
-- Terminate</t>
   </si>
   <si>
     <r>
@@ -518,10 +437,6 @@
     </r>
   </si>
   <si>
-    <t>Bot :
-Make note of it summary report</t>
-  </si>
-  <si>
     <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
 PeopleSoft app is unavailable. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
 Thanks,&lt;br&gt;
@@ -534,18 +449,12 @@
 Automation Team&lt;br&gt;</t>
   </si>
   <si>
-    <t>Business or Support Team Responsibility</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
     <t>Body</t>
   </si>
   <si>
-    <t>Recovery Steps If Applicable</t>
-  </si>
-  <si>
     <t>CC</t>
   </si>
   <si>
@@ -574,9 +483,6 @@
   </si>
   <si>
     <t>BE_4:Vouchers not available after filters and validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE_5: Pay group not available in "pay group" field  for Query # 6 PCARD_PAYGROUP_CH </t>
   </si>
   <si>
     <t>DatetimeFormat</t>
@@ -598,18 +504,320 @@
 Automation Team</t>
   </si>
   <si>
-    <t>End of the process</t>
+    <t>P001_090_PayCycleQueries_BotFolderName</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ManualFolderName</t>
+  </si>
+  <si>
+    <t>Name of the bot folder in sharepoint as well as local</t>
+  </si>
+  <si>
+    <t>Name of the manual folder in sharepoint as well as local</t>
+  </si>
+  <si>
+    <t>Query1Name</t>
+  </si>
+  <si>
+    <t>Query2Name</t>
+  </si>
+  <si>
+    <t>Query3Name</t>
+  </si>
+  <si>
+    <t>Query4Name</t>
+  </si>
+  <si>
+    <t>Query5Name</t>
+  </si>
+  <si>
+    <t>Query6Name</t>
+  </si>
+  <si>
+    <t>Query1RunID</t>
+  </si>
+  <si>
+    <t>Query2RunID</t>
+  </si>
+  <si>
+    <t>Query3RunID</t>
+  </si>
+  <si>
+    <t>Query4RunID</t>
+  </si>
+  <si>
+    <t>Query5RunID</t>
+  </si>
+  <si>
+    <t>Query6RunID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query1RunControlID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query3RunControlID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query4RunControlID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query5RunControlID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query6RunControlID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query2RunControlID</t>
+  </si>
+  <si>
+    <t>Name of the Run control ID of query 1</t>
+  </si>
+  <si>
+    <t>Name of the Run control ID of query 2</t>
+  </si>
+  <si>
+    <t>Name of the Run control ID of query 3</t>
+  </si>
+  <si>
+    <t>Name of the Run control ID of query 4</t>
+  </si>
+  <si>
+    <t>Name of the Run control ID of query 5</t>
+  </si>
+  <si>
+    <t>Name of the Run control ID of query 6</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query1Name</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query2Name</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query3Name</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query4Name</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query5Name</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_Query6Name</t>
+  </si>
+  <si>
+    <t>Name of query 1</t>
+  </si>
+  <si>
+    <t>Name of query 2</t>
+  </si>
+  <si>
+    <t>Name of query 3</t>
+  </si>
+  <si>
+    <t>Name of query 4</t>
+  </si>
+  <si>
+    <t>Name of query 5</t>
+  </si>
+  <si>
+    <t>Name of query 6</t>
+  </si>
+  <si>
+    <t>LocalFolder</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_LocalFolder</t>
+  </si>
+  <si>
+    <t>Full path of the local folder where files will be processed</t>
+  </si>
+  <si>
+    <t>TPStaff</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_TPStaff</t>
+  </si>
+  <si>
+    <t>The list of TP staff seperated by comma</t>
+  </si>
+  <si>
+    <t>SummaryPath</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_SummaryPath</t>
+  </si>
+  <si>
+    <t>The full path where the summary report will be saved in the local folder</t>
+  </si>
+  <si>
+    <t>StartEndTimeFormat</t>
+  </si>
+  <si>
+    <t>The format used to parse time from assets</t>
+  </si>
+  <si>
+    <t>MM-dd-yyyy h:mmtt</t>
+  </si>
+  <si>
+    <t>SE_3</t>
+  </si>
+  <si>
+    <t>SE_3: Duration drop down does not exist</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+Process Monitor refresh failed because the duration dropdown did not contain the value that was configured. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Automation support team: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Please correct the duration dropdown value prior to the next Bot run&lt;br&gt;&lt;br&gt;
+Thanks,&lt;br&gt;
+Automation Team
+</t>
+    </r>
+  </si>
+  <si>
+    <t>SE_4</t>
+  </si>
+  <si>
+    <t>SE_4: Navigation to Process Monitor failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+Navigation to Process Monitor failed as the application was not responsive. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
+Thanks,&lt;br&gt;
+Automation Team
+</t>
+  </si>
+  <si>
+    <t>PeoplesoftCredentialAssetFolder</t>
+  </si>
+  <si>
+    <t>This is the credential asset folder</t>
+  </si>
+  <si>
+    <t>SE_6</t>
+  </si>
+  <si>
+    <t>SE_6: Sharepoint folders not available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+The sharepoint site is unavailable for bot processing. Please validate the process automation folder and reach out to the automation team .&lt;br&gt;&lt;br&gt;
+Thanks,&lt;br&gt;
+Automation Team
+</t>
+  </si>
+  <si>
+    <t>DEV/P001_090_PayCycleQueries</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SE: Unexpected error occurred - {Exception Details}</t>
+  </si>
+  <si>
+    <t>Unexpected error occurred in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>PeopleSoft application unavailable in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>PeopleSoft login failed in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Duration drop down does not exist in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Navigation to Process Monitor failed in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Sharepoint folders not available in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Queries unavailable in Peoplesoft in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+The process faced an unexpected error. The error details are as follows&lt;br&gt;&lt;br&gt;
+&lt;u&gt;Error Details:&lt;/u&gt; {Exception Details}&lt;br&gt;&lt;br&gt;
+Thanks,&lt;br&gt;
+Automation Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -739,58 +947,73 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -815,9 +1038,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -855,7 +1078,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -961,7 +1184,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1103,7 +1326,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1111,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1164,18 +1387,18 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1184,7 +1407,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
@@ -1196,7 +1419,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>21</v>
@@ -1208,147 +1431,108 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>115</v>
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
+        <v>203</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>98</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
         <v>55</v>
       </c>
-    </row>
+      <c r="C14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-    </row>
+        <v>196</v>
+      </c>
+      <c r="C16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" t="s">
-        <v>79</v>
-      </c>
-    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2322,13 +2506,8 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3501,17 +3680,17 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3561,13 +3740,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3575,10 +3754,10 @@
         <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3586,235 +3765,456 @@
         <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="2" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -4762,359 +5162,337 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB048EB-7BC5-4528-AC4D-7EFC70AE54E8}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="7" width="49.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1">
+    <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>128</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="120">
-      <c r="A2" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="39.75" customHeight="1">
+      <c r="A2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="14"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="18" t="s">
+      <c r="D2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="39.75" customHeight="1">
+      <c r="A3" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="39.75" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45.75" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="L2" s="9"/>
-    </row>
-    <row r="3" spans="1:12" ht="120">
-      <c r="A3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="C5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" s="9" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="48" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="H6" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" customHeight="1">
+      <c r="A8" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="40.5" customHeight="1">
+      <c r="A9" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="L3" s="9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="195">
-      <c r="A4" s="8" t="s">
+      <c r="C11" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="135">
-      <c r="A5" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="45">
-      <c r="A6" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="45">
-      <c r="A7" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="45">
-      <c r="A8" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" ht="45">
-      <c r="A9" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="C12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated filter query for query 5
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415658C8-8297-44CD-8710-0833F61C6D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDBD6FB-8E55-491F-9BB7-3C4E1239F67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="221">
   <si>
     <t>Name</t>
   </si>
@@ -727,12 +727,6 @@
 </t>
   </si>
   <si>
-    <t>DEV/P001_090_PayCycleQueries</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>SE</t>
   </si>
   <si>
@@ -765,6 +759,15 @@
 &lt;u&gt;Error Details:&lt;/u&gt; {Exception Details}&lt;br&gt;&lt;br&gt;
 Thanks,&lt;br&gt;
 Automation Team</t>
+  </si>
+  <si>
+    <t>This is the path for the share point root folder where all files are saved</t>
+  </si>
+  <si>
+    <t>PROD/P001_090_PayCycleQueries</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1407,7 +1410,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
@@ -1445,7 +1448,7 @@
         <v>203</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>204</v>
@@ -1460,7 +1463,7 @@
         <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
         <v>99</v>
@@ -3687,10 +3690,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C35"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3746,7 +3749,7 @@
         <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3757,7 +3760,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3768,7 +3771,7 @@
         <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3779,7 +3782,10 @@
         <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3790,7 +3796,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>82</v>
@@ -3804,7 +3810,7 @@
         <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>82</v>
@@ -3818,7 +3824,7 @@
         <v>76</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>83</v>
@@ -3832,7 +3838,7 @@
         <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>83</v>
@@ -3846,7 +3852,7 @@
         <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>84</v>
@@ -3860,7 +3866,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>84</v>
@@ -3874,7 +3880,7 @@
         <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>87</v>
@@ -3888,7 +3894,7 @@
         <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>90</v>
@@ -3902,7 +3908,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>93</v>
@@ -3916,7 +3922,7 @@
         <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>104</v>
@@ -3930,7 +3936,7 @@
         <v>102</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>105</v>
@@ -3944,7 +3950,7 @@
         <v>107</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>108</v>
@@ -3958,7 +3964,7 @@
         <v>141</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>142</v>
@@ -3972,7 +3978,7 @@
         <v>145</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>147</v>
@@ -3986,7 +3992,7 @@
         <v>146</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>148</v>
@@ -4000,7 +4006,7 @@
         <v>161</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>167</v>
@@ -4014,7 +4020,7 @@
         <v>166</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>168</v>
@@ -4028,7 +4034,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>169</v>
@@ -4042,7 +4048,7 @@
         <v>163</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>170</v>
@@ -4056,7 +4062,7 @@
         <v>164</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>171</v>
@@ -4070,7 +4076,7 @@
         <v>165</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>172</v>
@@ -4084,7 +4090,7 @@
         <v>173</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>179</v>
@@ -4098,7 +4104,7 @@
         <v>174</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>180</v>
@@ -4112,7 +4118,7 @@
         <v>175</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>181</v>
@@ -4126,7 +4132,7 @@
         <v>176</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>182</v>
@@ -4140,7 +4146,7 @@
         <v>177</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>183</v>
@@ -4154,7 +4160,7 @@
         <v>178</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>184</v>
@@ -4168,7 +4174,7 @@
         <v>186</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>187</v>
@@ -4182,7 +4188,7 @@
         <v>189</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>190</v>
@@ -4196,7 +4202,7 @@
         <v>192</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>193</v>
@@ -5161,7 +5167,6 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5172,7 +5177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB048EB-7BC5-4528-AC4D-7EFC70AE54E8}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -5238,19 +5243,19 @@
     </row>
     <row r="3" spans="1:8" ht="39.75" customHeight="1">
       <c r="A3" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>115</v>
@@ -5273,7 +5278,7 @@
         <v>114</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>126</v>
@@ -5299,7 +5304,7 @@
         <v>114</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>125</v>
@@ -5325,7 +5330,7 @@
         <v>114</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>199</v>
@@ -5351,7 +5356,7 @@
         <v>114</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>202</v>
@@ -5377,7 +5382,7 @@
         <v>114</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>207</v>
@@ -5403,7 +5408,7 @@
         <v>119</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
Updated logic to deduct -1 and -3 days for refreshing process monitor
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1422861B-5E7A-473E-BABB-9AF4CFBC3897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D0D023-6A63-4861-B3EC-FDAADD00969B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
     <sheet name="Email" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="221">
   <si>
     <t>Name</t>
   </si>
@@ -89,11 +102,11 @@
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="12"/>
+    <phoneticPr fontId="13"/>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="12"/>
+    <phoneticPr fontId="13"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -298,15 +311,6 @@
   </si>
   <si>
     <t>UserID for Process Monitor fields</t>
-  </si>
-  <si>
-    <t>ProcessMonitorDurationType</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_ProcessMonitorDurationType</t>
-  </si>
-  <si>
-    <t>Duration type (Days, Weeks, Years)</t>
   </si>
   <si>
     <t>P001_090_PayCycleQueries_Query</t>
@@ -663,12 +667,87 @@
     <t>SE_3</t>
   </si>
   <si>
-    <t>SE_3: Duration drop down does not exist</t>
+    <t>SE_4</t>
+  </si>
+  <si>
+    <t>SE_4: Navigation to Process Monitor failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+Navigation to Process Monitor failed as the application was not responsive. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
+Thanks,&lt;br&gt;
+Automation Team
+</t>
+  </si>
+  <si>
+    <t>PeoplesoftCredentialAssetFolder</t>
+  </si>
+  <si>
+    <t>This is the credential asset folder</t>
+  </si>
+  <si>
+    <t>SE_6</t>
+  </si>
+  <si>
+    <t>SE_6: Sharepoint folders not available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+The sharepoint site is unavailable for bot processing. Please validate the process automation folder and reach out to the automation team .&lt;br&gt;&lt;br&gt;
+Thanks,&lt;br&gt;
+Automation Team
+</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SE: Unexpected error occurred - {Exception Details}</t>
+  </si>
+  <si>
+    <t>Unexpected error occurred in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>PeopleSoft application unavailable in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>PeopleSoft login failed in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Navigation to Process Monitor failed in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Sharepoint folders not available in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Queries unavailable in Peoplesoft in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+The process faced an unexpected error. The error details are as follows&lt;br&gt;&lt;br&gt;
+&lt;u&gt;Error Details:&lt;/u&gt; {Exception Details}&lt;br&gt;&lt;br&gt;
+Thanks,&lt;br&gt;
+Automation Team</t>
+  </si>
+  <si>
+    <t>This is the path for the share point root folder where all files are saved</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>SE_3: Date Range drop down does not exist</t>
+  </si>
+  <si>
+    <t>Date Range drop down does not exist in {Process Name} Process</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
-Process Monitor refresh failed because the duration dropdown did not contain the value that was configured. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
+Process Monitor refresh failed because the date range dropdown did not contain the value that was configured. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
 </t>
     </r>
     <r>
@@ -695,90 +774,31 @@
     </r>
   </si>
   <si>
-    <t>SE_4</t>
-  </si>
-  <si>
-    <t>SE_4: Navigation to Process Monitor failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
-Navigation to Process Monitor failed as the application was not responsive. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
-Thanks,&lt;br&gt;
-Automation Team
-</t>
-  </si>
-  <si>
-    <t>PeoplesoftCredentialAssetFolder</t>
-  </si>
-  <si>
-    <t>This is the credential asset folder</t>
-  </si>
-  <si>
-    <t>SE_6</t>
-  </si>
-  <si>
-    <t>SE_6: Sharepoint folders not available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
-The sharepoint site is unavailable for bot processing. Please validate the process automation folder and reach out to the automation team .&lt;br&gt;&lt;br&gt;
-Thanks,&lt;br&gt;
-Automation Team
-</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>SE: Unexpected error occurred - {Exception Details}</t>
-  </si>
-  <si>
-    <t>Unexpected error occurred in {Process Name} Process</t>
-  </si>
-  <si>
-    <t>PeopleSoft application unavailable in {Process Name} Process</t>
-  </si>
-  <si>
-    <t>PeopleSoft login failed in {Process Name} Process</t>
-  </si>
-  <si>
-    <t>Duration drop down does not exist in {Process Name} Process</t>
-  </si>
-  <si>
-    <t>Navigation to Process Monitor failed in {Process Name} Process</t>
-  </si>
-  <si>
-    <t>Sharepoint folders not available in {Process Name} Process</t>
-  </si>
-  <si>
-    <t>Queries unavailable in Peoplesoft in {Process Name} Process</t>
-  </si>
-  <si>
-    <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
-The process faced an unexpected error. The error details are as follows&lt;br&gt;&lt;br&gt;
-&lt;u&gt;Error Details:&lt;/u&gt; {Exception Details}&lt;br&gt;&lt;br&gt;
-Thanks,&lt;br&gt;
-Automation Team</t>
-  </si>
-  <si>
-    <t>This is the path for the share point root folder where all files are saved</t>
-  </si>
-  <si>
-    <t>PROD/P001_090_PayCycleQueries</t>
-  </si>
-  <si>
-    <t>PROD</t>
+    <t>ProcessMonitorRangeType</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ProcessMonitorRangeType</t>
+  </si>
+  <si>
+    <t>Duration type (Last, Date Range)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -950,64 +970,67 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1339,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1390,10 +1413,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -1401,7 +1424,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1409,8 +1432,9 @@
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>219</v>
+      <c r="B4" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
@@ -1440,18 +1464,19 @@
         <v>52</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>198</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1460,13 +1485,14 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>220</v>
+        <v>95</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>Constants!$B$19</f>
+        <v>DEV</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -1505,13 +1531,13 @@
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2510,7 +2536,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="12"/>
+  <phoneticPr fontId="13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2521,7 +2547,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2711,6 +2737,12 @@
       </c>
     </row>
     <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" t="s">
+        <v>214</v>
+      </c>
       <c r="C19" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3683,7 +3715,7 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="12"/>
+  <phoneticPr fontId="13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3692,8 +3724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3748,8 +3780,9 @@
       <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>219</v>
+      <c r="C2" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3759,8 +3792,9 @@
       <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>219</v>
+      <c r="C3" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3770,8 +3804,9 @@
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>219</v>
+      <c r="C4" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3781,11 +3816,12 @@
       <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>219</v>
+      <c r="C5" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3795,8 +3831,9 @@
       <c r="B6" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>219</v>
+      <c r="C6" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>82</v>
@@ -3809,8 +3846,9 @@
       <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>219</v>
+      <c r="C7" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>82</v>
@@ -3823,8 +3861,9 @@
       <c r="B8" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>219</v>
+      <c r="C8" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>83</v>
@@ -3837,8 +3876,9 @@
       <c r="B9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>219</v>
+      <c r="C9" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>83</v>
@@ -3851,8 +3891,9 @@
       <c r="B10" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>219</v>
+      <c r="C10" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>84</v>
@@ -3865,8 +3906,9 @@
       <c r="B11" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>219</v>
+      <c r="C11" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>84</v>
@@ -3879,8 +3921,9 @@
       <c r="B12" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>219</v>
+      <c r="C12" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>87</v>
@@ -3893,8 +3936,9 @@
       <c r="B13" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>219</v>
+      <c r="C13" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>90</v>
@@ -3902,72 +3946,77 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="2" t="s">
         <v>219</v>
       </c>
+      <c r="C14" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>93</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>219</v>
+        <v>104</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>219</v>
+        <v>138</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
@@ -3975,13 +4024,14 @@
         <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>219</v>
+        <v>142</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
@@ -3989,223 +4039,239 @@
         <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>219</v>
+        <v>143</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>219</v>
+        <v>158</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>219</v>
+        <v>163</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>219</v>
+        <v>159</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>219</v>
+        <v>160</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>219</v>
+        <v>161</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>219</v>
+        <v>162</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>219</v>
+        <v>170</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>219</v>
+        <v>171</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>219</v>
+        <v>172</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>219</v>
+        <v>173</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>219</v>
+        <v>174</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>219</v>
+        <v>175</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>219</v>
+        <v>183</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B34" t="s">
-        <v>189</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>219</v>
+        <v>186</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>219</v>
+        <v>189</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
@@ -5168,7 +5234,7 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="12"/>
+  <phoneticPr fontId="13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5178,7 +5244,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5195,297 +5261,297 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>131</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="39.75" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="8"/>
       <c r="D2" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="39.75" customHeight="1">
       <c r="A3" s="22" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="39.75" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45.75" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>215</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>213</v>
+        <v>111</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>216</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="40.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="30">
       <c r="A12" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H12" s="8"/>
     </row>

</xml_diff>

<commit_message>
Adjustment to send summary report only when a transaction is processed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D0D023-6A63-4861-B3EC-FDAADD00969B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7D18F9-92DA-421A-8857-1A07FF329258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -736,9 +736,6 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>SE_3: Date Range drop down does not exist</t>
   </si>
   <si>
@@ -781,6 +778,9 @@
   </si>
   <si>
     <t>Duration type (Last, Date Range)</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B9" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>199</v>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="B11" s="2" t="str">
         <f>Constants!$B$19</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="C11" t="s">
         <v>96</v>
@@ -2546,7 +2546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2741,7 +2741,7 @@
         <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -3724,7 +3724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="C2" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="C3" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="C4" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="C5" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>212</v>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="C6" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>82</v>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C7" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>82</v>
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C8" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>83</v>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="C9" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>83</v>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="C10" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>84</v>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="C11" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>84</v>
@@ -3923,7 +3923,7 @@
       </c>
       <c r="C12" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>87</v>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="C13" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>90</v>
@@ -3946,17 +3946,17 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" t="s">
         <v>218</v>
-      </c>
-      <c r="B14" t="s">
-        <v>219</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="C15" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>101</v>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="C16" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>102</v>
@@ -3998,7 +3998,7 @@
       </c>
       <c r="C17" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>105</v>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="C18" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>139</v>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="C19" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>144</v>
@@ -4043,7 +4043,7 @@
       </c>
       <c r="C20" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>145</v>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="C21" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>164</v>
@@ -4073,7 +4073,7 @@
       </c>
       <c r="C22" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>165</v>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C23" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>166</v>
@@ -4103,7 +4103,7 @@
       </c>
       <c r="C24" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>167</v>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="C25" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>168</v>
@@ -4133,7 +4133,7 @@
       </c>
       <c r="C26" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>169</v>
@@ -4148,7 +4148,7 @@
       </c>
       <c r="C27" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>176</v>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C28" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>177</v>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="C29" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>178</v>
@@ -4193,7 +4193,7 @@
       </c>
       <c r="C30" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>179</v>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="C31" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>180</v>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="C32" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>181</v>
@@ -4238,7 +4238,7 @@
       </c>
       <c r="C33" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>184</v>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="C34" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>187</v>
@@ -4268,7 +4268,7 @@
       </c>
       <c r="C35" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>DEV/P001_090_PayCycleQueries</v>
+        <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>190</v>
@@ -5390,16 +5390,16 @@
         <v>194</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>111</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>216</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>217</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
Edited to fix sharepoint link
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7D18F9-92DA-421A-8857-1A07FF329258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E24948-0718-4667-B4AF-42F1F5898392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="224">
   <si>
     <t>Name</t>
   </si>
@@ -781,6 +781,15 @@
   </si>
   <si>
     <t>PROD</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_SharepointPathAppend</t>
+  </si>
+  <si>
+    <t>SharedPathAppend</t>
+  </si>
+  <si>
+    <t>Value to be appended between root sharepoint path and folder path</t>
   </si>
 </sst>
 </file>
@@ -2546,7 +2555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3724,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4274,7 +4283,21 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" t="s">
+        <v>221</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>PROD/P001_090_PayCycleQueries</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated current time extraction to be converted to CST
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E24948-0718-4667-B4AF-42F1F5898392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EBBFA6-9290-4A70-B489-5D38FF205097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -780,16 +780,16 @@
     <t>Duration type (Last, Date Range)</t>
   </si>
   <si>
+    <t>P001_090_PayCycleQueries_SharepointPathAppend</t>
+  </si>
+  <si>
+    <t>SharedPathAppend</t>
+  </si>
+  <si>
+    <t>Value to be appended between root sharepoint path and folder path</t>
+  </si>
+  <si>
     <t>PROD</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_SharepointPathAppend</t>
-  </si>
-  <si>
-    <t>SharedPathAppend</t>
-  </si>
-  <si>
-    <t>Value to be appended between root sharepoint path and folder path</t>
   </si>
 </sst>
 </file>
@@ -2555,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2750,7 +2750,7 @@
         <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -3733,7 +3733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -4285,17 +4285,17 @@
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C36" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
         <v>PROD/P001_090_PayCycleQueries</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated to get summary file from sharepoint
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EBBFA6-9290-4A70-B489-5D38FF205097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30525A7-901B-4B2C-8A05-D8179F4CBC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="229">
   <si>
     <t>Name</t>
   </si>
@@ -787,6 +787,21 @@
   </si>
   <si>
     <t>Value to be appended between root sharepoint path and folder path</t>
+  </si>
+  <si>
+    <t>SharepointSummaryFolder</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_SharepointSummaryFolder</t>
+  </si>
+  <si>
+    <t>SharepointSummaryTemplateName</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_SharepointSummaryTemplateQuery</t>
+  </si>
+  <si>
+    <t>LocalSummaryFolderName</t>
   </si>
   <si>
     <t>PROD</t>
@@ -1372,7 +1387,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1566,7 +1581,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2556,7 +2578,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2750,7 +2772,7 @@
         <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -3734,7 +3756,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4298,8 +4320,30 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" t="s">
+        <v>224</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>PROD/P001_090_PayCycleQueries</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>225</v>
+      </c>
+      <c r="B38" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>PROD/P001_090_PayCycleQueries</v>
+      </c>
+    </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added 2 new parameters in refresh process monitor
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1843B07E-9D4E-43EC-8E3B-312B987255BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D312EF-5BAD-4417-BBDE-F8A28A451094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="252">
   <si>
     <t>Name</t>
   </si>
@@ -858,7 +858,25 @@
 Thanks,&lt;br&gt;</t>
   </si>
   <si>
-    <t>PROD</t>
+    <t>ProcessType</t>
+  </si>
+  <si>
+    <t>ProcessName</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ProcessType</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ProcessName</t>
+  </si>
+  <si>
+    <t>This is the process Type dropdown value for Process Monitor refresh</t>
+  </si>
+  <si>
+    <t>This is the process Name value value for Process Monitor refresh</t>
+  </si>
+  <si>
+    <t>DEV</t>
   </si>
 </sst>
 </file>
@@ -1525,7 +1543,7 @@
       </c>
       <c r="B4" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
@@ -1564,7 +1582,7 @@
       </c>
       <c r="B9" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>198</v>
@@ -1580,7 +1598,7 @@
       </c>
       <c r="B11" s="2" t="str">
         <f>Constants!$B$19</f>
-        <v>PROD</v>
+        <v>DEV</v>
       </c>
       <c r="C11" t="s">
         <v>96</v>
@@ -2846,7 +2864,7 @@
         <v>212</v>
       </c>
       <c r="B19" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -3830,7 +3848,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3887,7 +3905,7 @@
       </c>
       <c r="C2" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3899,7 +3917,7 @@
       </c>
       <c r="C3" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3911,7 +3929,7 @@
       </c>
       <c r="C4" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D4" t="s">
         <v>240</v>
@@ -3926,7 +3944,7 @@
       </c>
       <c r="C5" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>211</v>
@@ -3941,7 +3959,7 @@
       </c>
       <c r="C6" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>82</v>
@@ -3956,7 +3974,7 @@
       </c>
       <c r="C7" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>82</v>
@@ -3971,7 +3989,7 @@
       </c>
       <c r="C8" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>83</v>
@@ -3986,7 +4004,7 @@
       </c>
       <c r="C9" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>83</v>
@@ -4001,7 +4019,7 @@
       </c>
       <c r="C10" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>84</v>
@@ -4016,7 +4034,7 @@
       </c>
       <c r="C11" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>84</v>
@@ -4031,7 +4049,7 @@
       </c>
       <c r="C12" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>87</v>
@@ -4046,7 +4064,7 @@
       </c>
       <c r="C13" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>90</v>
@@ -4061,7 +4079,7 @@
       </c>
       <c r="C14" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>218</v>
@@ -4076,7 +4094,7 @@
       </c>
       <c r="C15" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>101</v>
@@ -4091,7 +4109,7 @@
       </c>
       <c r="C16" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>102</v>
@@ -4106,7 +4124,7 @@
       </c>
       <c r="C17" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>105</v>
@@ -4121,7 +4139,7 @@
       </c>
       <c r="C18" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>138</v>
@@ -4136,7 +4154,7 @@
       </c>
       <c r="C19" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>143</v>
@@ -4151,7 +4169,7 @@
       </c>
       <c r="C20" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>144</v>
@@ -4166,7 +4184,7 @@
       </c>
       <c r="C21" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>163</v>
@@ -4181,7 +4199,7 @@
       </c>
       <c r="C22" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>164</v>
@@ -4196,7 +4214,7 @@
       </c>
       <c r="C23" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>165</v>
@@ -4211,7 +4229,7 @@
       </c>
       <c r="C24" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>166</v>
@@ -4226,7 +4244,7 @@
       </c>
       <c r="C25" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>167</v>
@@ -4241,7 +4259,7 @@
       </c>
       <c r="C26" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>168</v>
@@ -4256,7 +4274,7 @@
       </c>
       <c r="C27" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>175</v>
@@ -4271,7 +4289,7 @@
       </c>
       <c r="C28" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>176</v>
@@ -4286,7 +4304,7 @@
       </c>
       <c r="C29" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>177</v>
@@ -4301,7 +4319,7 @@
       </c>
       <c r="C30" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>178</v>
@@ -4316,7 +4334,7 @@
       </c>
       <c r="C31" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>179</v>
@@ -4331,7 +4349,7 @@
       </c>
       <c r="C32" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>180</v>
@@ -4346,7 +4364,7 @@
       </c>
       <c r="C33" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>183</v>
@@ -4361,7 +4379,7 @@
       </c>
       <c r="C34" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>186</v>
@@ -4376,7 +4394,7 @@
       </c>
       <c r="C35" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>189</v>
@@ -4391,7 +4409,7 @@
       </c>
       <c r="C36" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>221</v>
@@ -4406,7 +4424,7 @@
       </c>
       <c r="C37" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>239</v>
@@ -4421,7 +4439,7 @@
       </c>
       <c r="C38" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D38" t="s">
         <v>238</v>
@@ -4436,7 +4454,7 @@
       </c>
       <c r="C39" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D39" t="s">
         <v>235</v>
@@ -4451,7 +4469,7 @@
       </c>
       <c r="C40" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D40" t="s">
         <v>236</v>
@@ -4466,14 +4484,42 @@
       </c>
       <c r="C41" s="2" t="str">
         <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
-        <v>PROD/P001_090_PayCycleQueries</v>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D41" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
+      </c>
+      <c r="D42" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>246</v>
+      </c>
+      <c r="B43" t="s">
+        <v>248</v>
+      </c>
+      <c r="C43" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$19,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
+      </c>
+      <c r="D43" t="s">
+        <v>250</v>
+      </c>
+    </row>
     <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>